<commit_message>
Testes para solicitar beneficios e atualizei kanban
</commit_message>
<xml_diff>
--- a/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
+++ b/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\UEL\Software_Engineer\Docs\I - Planejamento\Sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A9019-89D1-4C2E-818C-63EDC44ABFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4431BE84-9291-4FFC-B95E-115F1B371201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B04B963E-11FD-49DF-8DE1-BF515C305792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>TAREFA</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>T2, T8</t>
+  </si>
+  <si>
+    <t>1h+30min</t>
+  </si>
+  <si>
+    <t>50min+1h</t>
   </si>
 </sst>
 </file>
@@ -507,7 +513,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +565,9 @@
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -578,7 +586,9 @@
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Casos de testes com JUnit, planejamento atualizado, processos (descrição de papeis)
</commit_message>
<xml_diff>
--- a/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
+++ b/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\UEL\Software_Engineer\Docs\I - Planejamento\Sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4431BE84-9291-4FFC-B95E-115F1B371201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD87FC9A-D4F9-4061-B850-521D64AAA8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B04B963E-11FD-49DF-8DE1-BF515C305792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>TAREFA</t>
   </si>
@@ -143,10 +143,37 @@
     <t>T2, T8</t>
   </si>
   <si>
-    <t>1h+30min</t>
-  </si>
-  <si>
     <t>50min+1h</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>1h50</t>
+  </si>
+  <si>
+    <t>2h+1h30</t>
+  </si>
+  <si>
+    <t>2h+1h+30min+2h+1h+1h</t>
+  </si>
+  <si>
+    <t>7h30</t>
+  </si>
+  <si>
+    <t>3h30</t>
+  </si>
+  <si>
+    <t>40min+20min</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>30min+2h+1h+1h30</t>
+  </si>
+  <si>
+    <t>5h</t>
   </si>
 </sst>
 </file>
@@ -513,17 +540,17 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.109375" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -566,9 +593,11 @@
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -587,9 +616,11 @@
         <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -607,8 +638,12 @@
       <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -626,8 +661,12 @@
       <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -645,8 +684,12 @@
       <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -664,8 +707,12 @@
       <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -683,8 +730,12 @@
       <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -702,8 +753,12 @@
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -740,7 +795,9 @@
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Planejado x Executado concluido
</commit_message>
<xml_diff>
--- a/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
+++ b/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\UEL\Software_Engineer\Docs\I - Planejamento\Sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD87FC9A-D4F9-4061-B850-521D64AAA8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EC03E-76BC-4715-8912-5D79172B59C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B04B963E-11FD-49DF-8DE1-BF515C305792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>TAREFA</t>
   </si>
@@ -89,18 +89,12 @@
     <t>gastou hoje</t>
   </si>
   <si>
-    <t>Ana, Beatriz e Laís</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Refinamento do JAVA</t>
   </si>
   <si>
-    <t>Criação e integração da interface com HTML e JavaScript</t>
-  </si>
-  <si>
     <t>Fazer diagrama de Pacotes</t>
   </si>
   <si>
@@ -174,6 +168,24 @@
   </si>
   <si>
     <t>5h</t>
+  </si>
+  <si>
+    <t>1h+30min</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>1h+1h30</t>
+  </si>
+  <si>
+    <t>2h30</t>
+  </si>
+  <si>
+    <t>Ana, Laís e Beatriz &lt;3</t>
+  </si>
+  <si>
+    <t>Criação e integração da interface com HTML e CSS</t>
   </si>
 </sst>
 </file>
@@ -540,7 +552,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,12 +585,12 @@
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -593,15 +605,15 @@
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -613,18 +625,18 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -636,18 +648,18 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -659,18 +671,18 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -682,18 +694,18 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -705,18 +717,18 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -728,18 +740,18 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
@@ -754,51 +766,57 @@
         <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>

</xml_diff>

<commit_message>
Diagrama de classe e formulario dos casos dos de uso atualizados
</commit_message>
<xml_diff>
--- a/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
+++ b/Docs/I - Planejamento/Sprint_4/TabelaTarefas_Sprint4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\UEL\Software_Engineer\Docs\I - Planejamento\Sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EC03E-76BC-4715-8912-5D79172B59C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1EDB05-67ED-4260-87EC-2C3365AC9E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B04B963E-11FD-49DF-8DE1-BF515C305792}"/>
   </bookViews>
@@ -182,10 +182,10 @@
     <t>2h30</t>
   </si>
   <si>
-    <t>Ana, Laís e Beatriz &lt;3</t>
-  </si>
-  <si>
     <t>Criação e integração da interface com HTML e CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana, Laís e Beatriz </t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -809,7 +809,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>46</v>

</xml_diff>